<commit_message>
progress, and all code probably done
</commit_message>
<xml_diff>
--- a/vvs_2324_assignment_1/DiagramsAndTables/Tables.xlsx
+++ b/vvs_2324_assignment_1/DiagramsAndTables/Tables.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuyu\Desktop\VS\vvs_2324_assignment_1\DiagramsAndTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E24105-F30D-4DE9-80B9-6454D2F84AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C89329A8-20FE-4D9D-B448-E747637021F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{1AD62D08-6243-48D3-8DCE-EA2A8BDC5E1D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{1AD62D08-6243-48D3-8DCE-EA2A8BDC5E1D}"/>
   </bookViews>
   <sheets>
     <sheet name="EdgeCoverage" sheetId="1" r:id="rId1"/>
     <sheet name="PrimePath" sheetId="2" r:id="rId2"/>
     <sheet name="AllCouplingUse" sheetId="3" r:id="rId3"/>
+    <sheet name="LogicBasedCoverage" sheetId="4" r:id="rId4"/>
+    <sheet name="BaseChoiceCoverage" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="106">
   <si>
     <t>test case values
 (tree1,tree2)</t>
@@ -267,6 +269,96 @@
   </si>
   <si>
     <t>(9,10)</t>
+  </si>
+  <si>
+    <t>Last-def</t>
+  </si>
+  <si>
+    <t>First-use</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>{children,elem,i}</t>
+  </si>
+  <si>
+    <t>position/index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">proposePosition:{1,6,8}, delete:{10} </t>
+  </si>
+  <si>
+    <t>delete:{10,11}</t>
+  </si>
+  <si>
+    <t>children</t>
+  </si>
+  <si>
+    <t>delete:{1,6,11}, compact:{9}</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>this==other</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>other instance of Ntree</t>
+  </si>
+  <si>
+    <t>equalTrees()</t>
+  </si>
+  <si>
+    <t>delete:{6,11}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a </t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>predicate value</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>testOne()</t>
+  </si>
+  <si>
+    <t>not possible</t>
+  </si>
+  <si>
+    <t>testTwo()</t>
+  </si>
+  <si>
+    <t>testThree()</t>
+  </si>
+  <si>
+    <t>testFour()</t>
+  </si>
+  <si>
+    <t>predicate</t>
+  </si>
+  <si>
+    <t>Clause</t>
+  </si>
+  <si>
+    <t>expression</t>
+  </si>
+  <si>
+    <t>a || (b &amp;&amp; c)</t>
   </si>
 </sst>
 </file>
@@ -296,7 +388,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -304,11 +396,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -322,11 +440,65 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="38">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -413,50 +585,87 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0DD41AB1-843F-4E2E-963A-60E42E175D86}" name="Table1" displayName="Table1" ref="F5:J9" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0DD41AB1-843F-4E2E-963A-60E42E175D86}" name="Table1" displayName="Table1" ref="F5:J9" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
   <autoFilter ref="F5:J9" xr:uid="{0DD41AB1-843F-4E2E-963A-60E42E175D86}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{0D49707D-D514-4AEA-A32C-32C356C42902}" name="t" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{6C630DE2-BAA9-4492-A076-6F0419C501A3}" name="test case values_x000a_(tree1,tree2)" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{B7A75417-3EE3-47A0-B846-888F572F8FE2}" name="expected value" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{7B689658-CCC4-4818-94B3-8C9FCF7F8D80}" name="test path" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{5B7C2469-7D63-4D2E-9C3D-C175F37A2BAB}" name="requirements covered" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{0D49707D-D514-4AEA-A32C-32C356C42902}" name="t" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{6C630DE2-BAA9-4492-A076-6F0419C501A3}" name="test case values_x000a_(tree1,tree2)" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{B7A75417-3EE3-47A0-B846-888F572F8FE2}" name="expected value" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{7B689658-CCC4-4818-94B3-8C9FCF7F8D80}" name="test path" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{5B7C2469-7D63-4D2E-9C3D-C175F37A2BAB}" name="requirements covered" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium28" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{052E1C7C-EB16-4280-82F9-CA40BEE432BE}" name="Table2" displayName="Table2" ref="F3:H22" totalsRowShown="0" headerRowDxfId="10" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{052E1C7C-EB16-4280-82F9-CA40BEE432BE}" name="Table2" displayName="Table2" ref="F3:H22" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
   <autoFilter ref="F3:H22" xr:uid="{052E1C7C-EB16-4280-82F9-CA40BEE432BE}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{3B5276F1-1137-4613-A828-B088291370E1}" name="Node Edge" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{E33BC1B5-ED6B-48B6-B18A-3626B42A2F73}" name="Def" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{185DB522-8517-49A2-8916-D364461AE36D}" name="Use" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{3B5276F1-1137-4613-A828-B088291370E1}" name="Node Edge" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{E33BC1B5-ED6B-48B6-B18A-3626B42A2F73}" name="Def" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{185DB522-8517-49A2-8916-D364461AE36D}" name="Use" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{07E93BBB-7EB9-4B7A-83AF-67BFDF0B3009}" name="Table3" displayName="Table3" ref="K3:M22" totalsRowShown="0" headerRowDxfId="5" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{07E93BBB-7EB9-4B7A-83AF-67BFDF0B3009}" name="Table3" displayName="Table3" ref="K3:M22" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="K3:M22" xr:uid="{07E93BBB-7EB9-4B7A-83AF-67BFDF0B3009}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{24DA0711-D370-4E08-85F1-82F6CDCB0489}" name="Node Edge" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{54D3CF20-77C5-42FC-810F-C03E91064FB2}" name="Def" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{461C999B-137F-4EEB-8B01-9A3C93CA10B6}" name="Use" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{24DA0711-D370-4E08-85F1-82F6CDCB0489}" name="Node Edge" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{54D3CF20-77C5-42FC-810F-C03E91064FB2}" name="Def" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{461C999B-137F-4EEB-8B01-9A3C93CA10B6}" name="Use" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6D44C5C1-DAAB-44D6-A859-788663A2FED8}" name="Table4" displayName="Table4" ref="P3:R21" totalsRowShown="0" headerRowDxfId="4" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6D44C5C1-DAAB-44D6-A859-788663A2FED8}" name="Table4" displayName="Table4" ref="P3:R21" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="P3:R21" xr:uid="{6D44C5C1-DAAB-44D6-A859-788663A2FED8}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{5B12B632-8D2A-4D82-A8DE-138DDF9C7062}" name="Node Edge" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{FEAA365A-B0BC-4131-B552-8DF7AA47DD94}" name="Def" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{5A01D0CE-FB52-4D51-B8A2-5030206CF32D}" name="Use" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{5B12B632-8D2A-4D82-A8DE-138DDF9C7062}" name="Node Edge" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{FEAA365A-B0BC-4131-B552-8DF7AA47DD94}" name="Def" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{5A01D0CE-FB52-4D51-B8A2-5030206CF32D}" name="Use" dataDxfId="16"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4C51070E-4F43-4A89-9F99-C0A44ADF22F0}" name="Table5" displayName="Table5" ref="J26:L28" totalsRowShown="0" headerRowDxfId="11" dataDxfId="12">
+  <autoFilter ref="J26:L28" xr:uid="{4C51070E-4F43-4A89-9F99-C0A44ADF22F0}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{FD4C5A16-7155-4023-B1A3-B7D0B491A271}" name="Variable" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{B96E639E-69EF-4E72-B353-3E0606887B58}" name="Last-def" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{1AE7C604-4791-4FEE-9472-60E5E07E4D88}" name="First-use" dataDxfId="13"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3AB4663B-B0FB-4C1A-821C-314A4F8C97E0}" name="Table6" displayName="Table6" ref="L5:P13" totalsRowShown="0" headerRowDxfId="5" dataDxfId="6">
+  <autoFilter ref="L5:P13" xr:uid="{3AB4663B-B0FB-4C1A-821C-314A4F8C97E0}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{5328AC46-F2A5-4608-B0EA-8E3F7EF548AB}" name="a " dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{47B54CAA-D1CF-49AD-AF7A-28C9C7038C08}" name="b" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{B5D04C1A-6E9D-4178-9CB1-431060351000}" name="c" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{328E0237-F748-4D13-98BC-EC6D505F9EAC}" name="predicate value" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{D9D02444-C4DB-4983-8A96-085E464FED66}" name="Test" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{117D6293-40B8-495C-B5B6-D085D997E432}" name="Table7" displayName="Table7" ref="E4:F7" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="E4:F7" xr:uid="{117D6293-40B8-495C-B5B6-D085D997E432}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{EFD6F872-BFCE-4012-AB36-FBA7B0B2CC06}" name="Clause" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{FD970A59-8B8C-4A24-9F28-A1A55F4D1FD8}" name="expression" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1033,8 +1242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45498AC8-C2F9-4308-A744-07E038D46CEE}">
   <dimension ref="E2:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1043,8 +1252,8 @@
     <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.85546875" bestFit="1" customWidth="1"/>
@@ -1253,7 +1462,7 @@
         <v>35</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="P9" s="4" t="s">
         <v>41</v>
@@ -1639,76 +1848,373 @@
       <c r="H24" s="4"/>
     </row>
     <row r="25" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
     </row>
     <row r="26" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
+      <c r="J26" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="M26" s="4"/>
     </row>
     <row r="27" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
+      <c r="J27" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="L27" s="4" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="28" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
+      <c r="J28" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="29" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
     </row>
     <row r="30" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
     </row>
     <row r="31" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
     </row>
     <row r="32" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
-    </row>
-    <row r="33" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+    </row>
+    <row r="33" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
-    </row>
-    <row r="34" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+    </row>
+    <row r="34" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
-    </row>
-    <row r="35" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+    </row>
+    <row r="35" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
     </row>
-    <row r="36" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
     </row>
-    <row r="37" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="3">
+  <tableParts count="4">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FF8FBBE-A142-407C-AF22-F31563519A24}">
+  <dimension ref="E1:P14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="11.28515625" customWidth="1"/>
+    <col min="15" max="15" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E4" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E6" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E7" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="L8" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="L9" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E10" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="L11" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="L12" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="L13" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{896CF09C-83DA-4755-8458-68E402B6DB6C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="8.5703125" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>